<commit_message>
changed the way i'm getting the names for an more stable one
</commit_message>
<xml_diff>
--- a/Amazon_Scrappers/BestEletronicPricesAmazon.xlsx
+++ b/Amazon_Scrappers/BestEletronicPricesAmazon.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="195">
   <si>
     <t>Date</t>
   </si>
@@ -25,13 +25,13 @@
     <t>ProductPrice</t>
   </si>
   <si>
-    <t>2023-09-22 11:53</t>
+    <t>2023-09-24 17:03</t>
   </si>
   <si>
     <t>JBL, Fone de Ouvido in Ear, C50HI - Preto</t>
   </si>
   <si>
-    <t>R$ 34,90</t>
+    <t>R$ 33,99</t>
   </si>
   <si>
     <t>Fire TV Stick Lite | Streaming em Full HD com Alexa | Com Controle Remoto Lite por Voz com Alexa (sem controles de TV)</t>
@@ -43,7 +43,7 @@
     <t>Celular Xiaomi Redmi Note 12 128GB / 6GB RAM/Dual Sim/TelaP e 13MP - Onyx Gray - Preto</t>
   </si>
   <si>
-    <t>R$ 997,45</t>
+    <t>R$ 976,77</t>
   </si>
   <si>
     <t>Smartphone Xiaomi Note 12 4G 128GB - 8GB Ram (Versao Global) (Onyx Gray)</t>
@@ -61,7 +61,19 @@
     <t>Pilha Alcalina AA Pequena DURACELL Com 16 Unidades</t>
   </si>
   <si>
-    <t>R$ 67,99</t>
+    <t>R$ 66,90</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Note 12S 256GB - 8GB Ram (Versao Global) (Onyx Black)</t>
+  </si>
+  <si>
+    <t>R$ 1.249,46</t>
+  </si>
+  <si>
+    <t>Novo Echo Dot 5ª geração | O Echo Dot com o melhor som já lançado | Cor Preta</t>
+  </si>
+  <si>
+    <t>R$ 429,00</t>
   </si>
   <si>
     <t>Clamper Energia 5 Tomadas</t>
@@ -70,15 +82,15 @@
     <t>R$ 54,00</t>
   </si>
   <si>
-    <t>Smartphone Xiaomi Note 12S 256GB - 8GB Ram (Versao Global) (Onyx Black)</t>
-  </si>
-  <si>
-    <t>R$ 1.262,95</t>
-  </si>
-  <si>
     <t>DURACELL - Pilha Alcalina AAA, Palito com 16 unidades</t>
   </si>
   <si>
+    <t>Smartphone Xiaomi Note 12 4G 128GB 6GB Ram (VERSAO GLOBAL) (Ice Blue)</t>
+  </si>
+  <si>
+    <t>R$ 983,57</t>
+  </si>
+  <si>
     <t>Suporte Fixo Universal de Parede Para TVs de 14” a 84” Até 100 kg - GENIUS ELG</t>
   </si>
   <si>
@@ -88,31 +100,61 @@
     <t>Smartphone Xiaomi POCO X5 Pro 5G Dual SIM 8GB 256GB 6,67" FHD+ 108MP 5000mAh 67W Carregamento (Preto)</t>
   </si>
   <si>
-    <t>R$ 1.815,54</t>
-  </si>
-  <si>
-    <t>Novo Echo Dot 5ª geração | O Echo Dot com o melhor som já lançado | Cor Preta</t>
-  </si>
-  <si>
-    <t>R$ 429,00</t>
+    <t>R$ 1.815,00</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Redmi 12C 128GB - 4GB Ram (Cinza)</t>
+  </si>
+  <si>
+    <t>R$ 689,99</t>
+  </si>
+  <si>
+    <t>JBL, Fone de Ouvido Sem Fio, Bluetooth, Wave Buds TWS - Preto</t>
+  </si>
+  <si>
+    <t>R$ 244,00</t>
+  </si>
+  <si>
+    <t>Mini Projetor Portatil 5G Wifi 6 Bluetooth 5.0 Android 11, Projetor 4K 1080P Full HD Suporte 8000 Lumens, Projetor Led Auto de Correcção Trapezóide Horizontal, 180°Girável Projector para Telefónico (EU Plug)</t>
+  </si>
+  <si>
+    <t>R$ 383,91</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Redmi Note 12 Pro 5G Dual SIM 256GB - 8GB Ram (Versao Global) (Midnight black)</t>
+  </si>
+  <si>
+    <t>R$ 1.760,00</t>
+  </si>
+  <si>
+    <t>Fone de Ouvido Bluetooth 5.0 Par Sem Fio Duplo - Intra Auricular MIURI</t>
+  </si>
+  <si>
+    <t>R$ 36,99</t>
+  </si>
+  <si>
+    <t>Suporte para TV Universal 14 a 84 fixo de parede UNI100 Elg</t>
+  </si>
+  <si>
+    <t>R$ 16,43</t>
   </si>
   <si>
     <t>PHILIPS Fone de ouvido sem fio TWS bluetooth com microfone e energia para 18 horas totais na cor preto, padrão, TAT1235BK/97</t>
   </si>
   <si>
-    <t>R$ 123,51</t>
-  </si>
-  <si>
-    <t>Smartphone Xiaomi Note 12 4G 128GB 6GB Ram (VERSAO GLOBAL) (Ice Blue)</t>
-  </si>
-  <si>
-    <t>R$ 1.002,30</t>
-  </si>
-  <si>
-    <t>JBL, Fone de Ouvido Sem Fio, Bluetooth, Wave Buds TWS - Preto</t>
-  </si>
-  <si>
-    <t>R$ 248,00</t>
+    <t>R$ 169,90</t>
+  </si>
+  <si>
+    <t>Pilha Alcalina AAA com 8 unidades Elgin Palito</t>
+  </si>
+  <si>
+    <t>R$ 14,67</t>
+  </si>
+  <si>
+    <t>Smart TV LED 32'' HD Samsung LH32BETBLGGXZD</t>
+  </si>
+  <si>
+    <t>R$ 1.078,90</t>
   </si>
   <si>
     <t>Fone de Ouvido Philips com Microfone - Preto</t>
@@ -121,199 +163,442 @@
     <t>R$ 24,90</t>
   </si>
   <si>
-    <t>Mini Projetor Portatil 5G Wifi 6 Bluetooth 5.0 Android 11, Projetor 4K 1080P Full HD Suporte 8000 Lumens, Projetor Led Auto de Correcção Trapezóide Horizontal, 180°Girável Projector para Telefónico (EU Plug)</t>
-  </si>
-  <si>
-    <t>R$ 389,90</t>
+    <t>Antena de TV Interna UHF/HDTV AI 2031 Intelbras</t>
+  </si>
+  <si>
+    <t>R$ 29,90</t>
+  </si>
+  <si>
+    <t>Apresentamos o Echo Pop | Smart speaker compacto com som envolvente e Alexa | Cor Preta</t>
+  </si>
+  <si>
+    <t>Pilha recarregável AAA 1000mAh Elgin com 4 unidades Palito</t>
+  </si>
+  <si>
+    <t>R$ 19,00</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Note 12S 256GB - 8GB Ram (Versao Global) (Ice Blue)</t>
+  </si>
+  <si>
+    <t>R$ 1.222,00</t>
   </si>
   <si>
     <t>Smartphone Xiaomi Redmi 12C 128GB - 4GB Ram (VERSAO GLOBAL) (Mint Green)</t>
   </si>
   <si>
+    <t>R$ 687,37</t>
+  </si>
+  <si>
+    <t>Xiaomi POCO X5 5G Smartphone Dual Sim 256GB Memory 8GB RAM 6.67" AMOLED Display 5000mAh 48MP+13MP CAM (preto)</t>
+  </si>
+  <si>
+    <t>R$ 1.469,99</t>
+  </si>
+  <si>
+    <t>Vaporizador Portátil Black Decker BDV2000V 1200W - 127V</t>
+  </si>
+  <si>
+    <t>R$ 188,50</t>
+  </si>
+  <si>
+    <t>Impressora Multifuncional HP Ink Tank 416 Original Tanque de Tinta Continua Wi-Fi Scanner de banda dupla. Funções: Imprimir, Copiar, Digitalizar. Cor ‎Preto (Z4B55A)</t>
+  </si>
+  <si>
+    <t>R$ 679,00</t>
+  </si>
+  <si>
+    <t>Protetor Eletrônico com 5 tomadas EPE 205 Preto Intelbras</t>
+  </si>
+  <si>
+    <t>R$ 35,00</t>
+  </si>
+  <si>
+    <t>Pilha Alcalina AA Elgin com 4 unidades Comum</t>
+  </si>
+  <si>
+    <t>R$ 7,49</t>
+  </si>
+  <si>
+    <t>Epson EcoTank L3250 - Multifuncional, Tanque de Tinta Colorida, Wi-Fi Direct, USB, Bivolt, Preto</t>
+  </si>
+  <si>
+    <t>R$ 1.122,01</t>
+  </si>
+  <si>
+    <t>Force Line - Extensão Slim, 3 Tomadas, Bipolar, Bivolt, 1 Metro, Branco</t>
+  </si>
+  <si>
+    <t>R$ 8,99</t>
+  </si>
+  <si>
+    <t>Fone de ouvido sem fio QCY T13 TWS Bluetooth 5.1 com 4 microfones Touch Control IPX5 à prova d'água 40 horas de tempo de reprodução</t>
+  </si>
+  <si>
+    <t>R$ 129,00</t>
+  </si>
+  <si>
+    <t>DURACELL - Carregador de Pilhas Recarregáveis AA e AAA Com 4 Pilhas AA</t>
+  </si>
+  <si>
+    <t>R$ 164,90</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Note 12 4G 128GB 6GB Ram (VERSAO GLOBAL) (Mint Green)</t>
+  </si>
+  <si>
+    <t>R$ 1.004,76</t>
+  </si>
+  <si>
+    <t>JBL, Headset Gamer, Quantum 100 - Preto</t>
+  </si>
+  <si>
+    <t>R$ 138,00</t>
+  </si>
+  <si>
+    <t>Samsung Book Intel® Core™ i5-1135G7, Windows 11 Home, 8GB, 256GB SSD, Intel Iris Xe, 15.6'' Full HD LED, NP550XDA-KH2BR</t>
+  </si>
+  <si>
+    <t>R$ 2.679,90</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi POCO X5 Pro 5G Dual SIM 8GB 256GB 6,67" FHD+ 108MP 5000mAh 67W Carregamento (Azul)</t>
+  </si>
+  <si>
+    <t>R$ 1.831,00</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Redmi Note 12S Onyx Black 8GB Ram 256GB</t>
+  </si>
+  <si>
+    <t>R$ 1.229,25</t>
+  </si>
+  <si>
+    <t>Protetor Eletrônico com 5 tomadas EPE 1005+ Branco Intelbras</t>
+  </si>
+  <si>
+    <t>R$ 28,00</t>
+  </si>
+  <si>
+    <t>Haiz Smartwatch Relógio Inteligente IP67 44mm My Watch I Fit PRETO HZ-ZL02D</t>
+  </si>
+  <si>
+    <t>R$ 175,49</t>
+  </si>
+  <si>
+    <t>Wifi Hd 1080p A8 Câmera de Segurança, Câmera Ip Icsee Prova D'água Infravermelho Externa（Smartcamera-A08）</t>
+  </si>
+  <si>
+    <t>R$ 99,00</t>
+  </si>
+  <si>
+    <t>Smart TV LED 43" Full HD Samsung LH43BETMLGGXZD, 2 HDMI, 1 USB, Wi-Fi, HDR, Sistema Operacional Tizen e Dolby Digital Plus</t>
+  </si>
+  <si>
+    <t>R$ 1.599,00</t>
+  </si>
+  <si>
+    <t>Novo Fire TV Stick 4K | Streaming com Dolby Vision/Atmos e suporte a wi-fi 6 | Com Alexa e comandos de TV</t>
+  </si>
+  <si>
     <t>R$ 449,00</t>
   </si>
   <si>
-    <t>Epson EcoTank L3250 - Multifuncional, Tanque de Tinta Colorida, Wi-Fi Direct, USB, Bivolt, Preto</t>
-  </si>
-  <si>
-    <t>R$ 684,00</t>
-  </si>
-  <si>
-    <t>Smartphone Xiaomi Redmi Note 12 Pro 5G Dual SIM 256GB - 8GB Ram (Versao Global) (Midnight black)</t>
-  </si>
-  <si>
-    <t>R$ 953,67</t>
-  </si>
-  <si>
-    <t>Smart TV LED 32'' HD Samsung LH32BETBLGGXZD</t>
-  </si>
-  <si>
-    <t>R$ 1.760,00</t>
-  </si>
-  <si>
-    <t>Vaporizador Portátil Black Decker BDV2000V 1200W - 127V</t>
-  </si>
-  <si>
-    <t>R$ 1.078,90</t>
-  </si>
-  <si>
-    <t>Fone de Ouvido Bluetooth 5.0 Par Sem Fio Duplo - Intra Auricular MIURI</t>
-  </si>
-  <si>
-    <t>R$ 181,41</t>
-  </si>
-  <si>
-    <t>Smartphone Xiaomi Redmi 12C 128GB - 4GB Ram (Cinza)</t>
-  </si>
-  <si>
-    <t>R$ 39,90</t>
-  </si>
-  <si>
-    <t>Samsung Book Intel® Core™ i5-1135G7, Windows 11 Home, 8GB, 256GB SSD, Intel Iris Xe, 15.6'' Full HD LED, NP550XDA-KH2BR</t>
-  </si>
-  <si>
-    <t>R$ 693,00</t>
+    <t>Samsung Smart TV Crystal 43" 4K UHD CU7700 - Alexa built in, Samsung Gaming Hub</t>
+  </si>
+  <si>
+    <t>R$ 1.905,49</t>
+  </si>
+  <si>
+    <t>Câmera Inteligente Interna Compatível com Alexa Wi-fi Full HD iM3 C Branca Intelbras</t>
+  </si>
+  <si>
+    <t>R$ 207,00</t>
+  </si>
+  <si>
+    <t>HP 2774 DeskJet Ink Advantage - Impressora Multifuncional, Wi-Fi, Scanner, Tecnologia de Impressão HP Thermal Inkjet, Funções: Impressão, Cópia, Digitalização</t>
+  </si>
+  <si>
+    <t>R$ 319,00</t>
+  </si>
+  <si>
+    <t>JBL, Fone de Ouvido On ear, Tune 520BT - Azul</t>
+  </si>
+  <si>
+    <t>R$ 239,00</t>
+  </si>
+  <si>
+    <t>Celular Xiaomi Redmi 12C 128GB / 4GB RAM/Dual Sim/Tela 6.71" / Câmeras 50MP+0.08MP e 5MP - Graphite Gray (Global)</t>
+  </si>
+  <si>
+    <t>R$ 695,66</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Redmi 12C 128GB - 4GB Ram Ocean Blue (AZUL) (Azul)</t>
+  </si>
+  <si>
+    <t>R$ 689,00</t>
+  </si>
+  <si>
+    <t>Monitor LG 19.5'' LED HD - HDMI, 2ms, Ajuste de Inclinação, Reader Mode, 4-Screen Split, - 20MK400H-B</t>
+  </si>
+  <si>
+    <t>R$ 398,89</t>
+  </si>
+  <si>
+    <t>HD SSD Kingston SA400S37 480GB</t>
+  </si>
+  <si>
+    <t>R$ 164,80</t>
   </si>
   <si>
     <t>SAMSUNG GALAXY BUDS 2 PRETO, Pequeno, SM-R177</t>
   </si>
   <si>
-    <t>R$ 2.679,90</t>
-  </si>
-  <si>
-    <t>Impressora Multifuncional HP Ink Tank 416 Original Tanque de Tinta Continua Wi-Fi Scanner de banda dupla. Funções: Imprimir, Copiar, Digitalizar. Cor ‎Preto (Z4B55A)</t>
-  </si>
-  <si>
-    <t>R$ 279,00</t>
-  </si>
-  <si>
-    <t>Xiaomi POCO X5 5G Smartphone Dual Sim 256GB Memory 8GB RAM 6.67" AMOLED Display 5000mAh 48MP+13MP CAM (preto)</t>
-  </si>
-  <si>
-    <t>R$ 679,00</t>
-  </si>
-  <si>
-    <t>Force Line - Extensão Slim, 3 Tomadas, Bipolar, Bivolt, 1 Metro, Branco</t>
-  </si>
-  <si>
-    <t>R$ 1.470,00</t>
-  </si>
-  <si>
-    <t>JBL, Headset Gamer, Quantum 100 - Preto</t>
-  </si>
-  <si>
-    <t>R$ 8,99</t>
-  </si>
-  <si>
-    <t>Protetor Eletrônico com 5 tomadas EPE 205 Preto Intelbras</t>
-  </si>
-  <si>
-    <t>R$ 134,42</t>
-  </si>
-  <si>
-    <t>Smartphone Xiaomi Note 12S 256GB - 8GB Ram (Versao Global) (Ice Blue)</t>
-  </si>
-  <si>
-    <t>R$ 35,00</t>
-  </si>
-  <si>
-    <t>Apresentamos o Echo Pop | Smart speaker compacto com som envolvente e Alexa | Cor Preta</t>
-  </si>
-  <si>
-    <t>R$ 1.220,00</t>
-  </si>
-  <si>
-    <t>Smartphone Xiaomi Note 12 4G 128GB 6GB Ram (VERSAO GLOBAL) (Mint Green)</t>
-  </si>
-  <si>
-    <t>Pilha recarregável AAA 1000mAh Elgin com 4 unidades Palito</t>
-  </si>
-  <si>
-    <t>R$ 1.012,16</t>
-  </si>
-  <si>
-    <t>Antena de TV Interna UHF/HDTV AI 2031 Intelbras</t>
-  </si>
-  <si>
-    <t>R$ 19,00</t>
-  </si>
-  <si>
-    <t>Pilha Alcalina AAA com 8 unidades Elgin Palito</t>
-  </si>
-  <si>
-    <t>R$ 29,90</t>
-  </si>
-  <si>
-    <t>Suporte para TV Universal 14 a 84 fixo de parede UNI100 Elg</t>
-  </si>
-  <si>
-    <t>R$ 14,67</t>
-  </si>
-  <si>
-    <t>Smartphone Xiaomi Redmi 12C 128GB - 4GB Ram Ocean Blue (AZUL) (Azul)</t>
-  </si>
-  <si>
-    <t>R$ 16,43</t>
-  </si>
-  <si>
-    <t>HP 2774 DeskJet Ink Advantage - Impressora Multifuncional, Wi-Fi, Scanner, Tecnologia de Impressão HP Thermal Inkjet, Funções: Impressão, Cópia, Digitalização</t>
-  </si>
-  <si>
-    <t>R$ 682,41</t>
-  </si>
-  <si>
-    <t>Câmera Inteligente Interna Compatível com Alexa Wi-fi Full HD iM3 C Branca Intelbras</t>
-  </si>
-  <si>
-    <t>R$ 319,00</t>
-  </si>
-  <si>
-    <t>Haiz Smartwatch Relógio Inteligente IP67 44mm My Watch I Fit PRETO HZ-ZL02D</t>
-  </si>
-  <si>
-    <t>R$ 207,00</t>
-  </si>
-  <si>
-    <t>DURACELL - Carregador de Pilhas Recarregáveis AA e AAA Com 4 Pilhas AA</t>
-  </si>
-  <si>
-    <t>R$ 175,49</t>
-  </si>
-  <si>
-    <t>Wifi Hd 1080p A8 Câmera de Segurança, Câmera Ip Icsee Prova D'água Infravermelho Externa（Smartcamera-A08）</t>
-  </si>
-  <si>
-    <t>R$ 164,90</t>
-  </si>
-  <si>
-    <t>Pilha Alcalina AA Elgin com 4 unidades Comum</t>
-  </si>
-  <si>
-    <t>R$ 99,00</t>
-  </si>
-  <si>
-    <t>Smartphone Xiaomi POCO X5 Pro 5G Dual SIM 8GB 256GB 6,67" FHD+ 108MP 5000mAh 67W Carregamento (Azul)</t>
-  </si>
-  <si>
-    <t>R$ 7,49</t>
-  </si>
-  <si>
-    <t>Smartphone Xiaomi Redmi Note 12S Onyx Black 8GB Ram 256GB</t>
-  </si>
-  <si>
-    <t>R$ 1.831,60</t>
-  </si>
-  <si>
-    <t>Samsung Smart TV Crystal 43" 4K UHD CU7700 - Alexa built in, Samsung Gaming Hub</t>
-  </si>
-  <si>
-    <t>R$ 1.240,00</t>
+    <t>R$ 297,00</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Note 12S 256GB - 8GB Ram (Versao Global) (Pearl Green)</t>
+  </si>
+  <si>
+    <t>R$ 1.250,00</t>
+  </si>
+  <si>
+    <t>Suporte Fixo de Parede Para TVs de 32"a 65" com Peso até 50kg - N01V4 ELG</t>
+  </si>
+  <si>
+    <t>R$ 51,98</t>
+  </si>
+  <si>
+    <t>Adaptador de energia</t>
+  </si>
+  <si>
+    <t>Apple iPhone 13 (128 GB) - Meia-noite</t>
+  </si>
+  <si>
+    <t>R$ 4.377,00</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Redmi 12 4G 256GB - 8GB Ram (Versao Global) (Midnight Black)</t>
+  </si>
+  <si>
+    <t>R$ 1.137,71</t>
+  </si>
+  <si>
+    <t>Headphone Philips bluetooth on-ear com microfone e energia para 15 horas na cor preto TAH1108BK/55</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Redmi Note 12 Pro 5G Dual SIM 256GB - 8GB Ram (Versao Global) (Sky Blue)</t>
+  </si>
+  <si>
+    <t>R$ 1.775,24</t>
   </si>
   <si>
     <t>Smart TV 32” Philco PTV32G7ER2CPBLH Dolby Audio Led Bivolt</t>
   </si>
   <si>
-    <t>R$ 1.898,90</t>
+    <t>R$ 929,90</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Poco F5 com processador Snapdragon 7+ Gen 2 Dual SIM 5G 12gb Ram 256gb Rom (Black)</t>
+  </si>
+  <si>
+    <t>R$ 2.380,00</t>
+  </si>
+  <si>
+    <t>Fone De Ouvido Sem Fio 5.0 Display Headset Compatível com todos os aparelhos</t>
+  </si>
+  <si>
+    <t>R$ 23,39</t>
+  </si>
+  <si>
+    <t>SAMSUNG Smart TV Crystal 50" 4K UHD CU7700 - Alexa built in, Samsung Gaming Hub</t>
+  </si>
+  <si>
+    <t>R$ 2.099,00</t>
+  </si>
+  <si>
+    <t>Controle remoto universal para todos os televisores Samsung, substituição para todos os televisores LCD LED HDTV 3D Smart Samsung</t>
+  </si>
+  <si>
+    <t>R$ 8,00</t>
+  </si>
+  <si>
+    <t>Câmera IP Sem Fio de Segurança Externa HD 4MP, Câmera de Visão Noturna Infravermelha WiFi, IP66 à Prova D'água e à Prova de Poeira, Chamada de Voz Bidirecional, Campo de Visão Completo PTZ 360 Graus, Detecção de Movimento</t>
+  </si>
+  <si>
+    <t>R$ 159,99</t>
+  </si>
+  <si>
+    <t>Mini Projetor Portatil WiFi 5G Bluetooth 5.0,Salange Hy300 Smart Projetor Android 11, 8500 Lúmens Projetor LED 4K 1080P Full HD Suporte (EU Plug)</t>
+  </si>
+  <si>
+    <t>R$ 389,98</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Redmi Note 12 Pro 5G Dual SIM 256GB - 8GB Ram (Versao Global) (Polar White)</t>
+  </si>
+  <si>
+    <t>R$ 1.797,00</t>
+  </si>
+  <si>
+    <t>Xiaomi POCO X5 5G Smartphone Dual Sim 256GB Memory 8GB RAM 6.67" AMOLED Display 5000mAh 48MP+13MP CAM (verde)</t>
+  </si>
+  <si>
+    <t>R$ 1.447,63</t>
+  </si>
+  <si>
+    <t>Novo Echo Dot 5ª geração | O Echo Dot com o melhor som já lançado | Cor Azul</t>
+  </si>
+  <si>
+    <t>Pilha recarregável AA 2700Mah Elgin Com 4 unidades Comum</t>
+  </si>
+  <si>
+    <t>R$ 37,00</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi POCO X5 Pro 5G Dual SIM 6GB 128GB 6,67" FHD+ 108MP 5000mAh 67W Carregamento (Preto)</t>
+  </si>
+  <si>
+    <t>R$ 1.697,26</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Poco M5 128GB 6Gb Black no Brasil - Preto</t>
+  </si>
+  <si>
+    <t>R$ 893,00</t>
+  </si>
+  <si>
+    <t>Roku Express - Streaming player Full HD, Transforma sua TV em Smart TV, Com controle remoto e cabo HDMI incluídos</t>
+  </si>
+  <si>
+    <t>R$ 200,61</t>
+  </si>
+  <si>
+    <t>Adaptador Tomada Universal Padrão Internacional 150 Países Viagem Bivolt</t>
+  </si>
+  <si>
+    <t>R$ 5,54</t>
+  </si>
+  <si>
+    <t>SSD Kingston NV2 1TB NVMe M.2 2280 (Leitura até 3500MB/s e Gravação até 2100MB/s)</t>
+  </si>
+  <si>
+    <t>R$ 287,90</t>
+  </si>
+  <si>
+    <t>JBL, Fone de Ouvido On ear, Tune 520BT - Preto</t>
+  </si>
+  <si>
+    <t>R$ 236,00</t>
+  </si>
+  <si>
+    <t>Smartphone Redmi 12 4G 128GB - 4GB Ram (Versao Global) (Sky Blue)</t>
+  </si>
+  <si>
+    <t>R$ 927,63</t>
+  </si>
+  <si>
+    <t>PILHA EVEREADY SM-PALITO AAA4</t>
+  </si>
+  <si>
+    <t>R$ 8,72</t>
+  </si>
+  <si>
+    <t>Adaptador/Conversor HDMI para VGA com Áudio</t>
+  </si>
+  <si>
+    <t>R$ 13,90</t>
+  </si>
+  <si>
+    <t>Fones de ouvido sem fio TWS JBL Wave Flex - Branco - JBLWFLEXWHT</t>
+  </si>
+  <si>
+    <t>R$ 335,00</t>
+  </si>
+  <si>
+    <t>Smart TV LED, 50", Ultra HD 4K, LH50BETHVGGXZD, Samsung, 2HDMI, 1USB, Wifi</t>
+  </si>
+  <si>
+    <t>Edifier W800BT PLUS - Fone de Ouvido Headset, Bluetooth 5.1, Preto</t>
+  </si>
+  <si>
+    <t>R$ 289,99</t>
+  </si>
+  <si>
+    <t>Controle Remoto Tv Samsung Smart</t>
+  </si>
+  <si>
+    <t>R$ 10,50</t>
+  </si>
+  <si>
+    <t>Novo Echo Dot 5ª geração com Relógio | Smart speaker com Alexa | Cor Branca</t>
+  </si>
+  <si>
+    <t>R$ 529,00</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Note 12 Pro 4G - 256GB + 8GB Ram (Versao Global) (Graphite Gray)</t>
+  </si>
+  <si>
+    <t>R$ 1.299,00</t>
+  </si>
+  <si>
+    <t>Apple iPhone 13 (128 GB) - Luz das estrelas</t>
+  </si>
+  <si>
+    <t>R$ 4.443,33</t>
+  </si>
+  <si>
+    <t>Panasonic UM-3SHSL8P6, Pilha Comum Linha Super Hyper Proteção Antivazamento, pacote de 8</t>
+  </si>
+  <si>
+    <t>R$ 8,57</t>
+  </si>
+  <si>
+    <t>JBL, Fone de Ouvido Bluetooth, Tune 125 BT - Preto</t>
+  </si>
+  <si>
+    <t>R$ 160,35</t>
+  </si>
+  <si>
+    <t>Echo Dot (3ª Geração): Smart Speaker com Alexa - Cor Preta</t>
+  </si>
+  <si>
+    <t>R$ 1.147,00</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Redmi 12 4G 256GB - 8GB Ram (Versao Global) (Sky Blue)</t>
+  </si>
+  <si>
+    <t>R$ 51,00</t>
+  </si>
+  <si>
+    <t>Câmera Lâmpada de Segurança WiFi 1080P Visão Noturna Infravermelha bidirecional Giratoria 360 Yoosee</t>
+  </si>
+  <si>
+    <t>Impressora Epson Ecotank L121 - Tanque de Tinta Colorida, Cabo USB, Bivolt</t>
+  </si>
+  <si>
+    <t>R$ 1.126,43</t>
+  </si>
+  <si>
+    <t>Smartphone Motorola Moto G53 5G 128GB 4GB RAM Grafite</t>
+  </si>
+  <si>
+    <t>R$ 2.246,00</t>
+  </si>
+  <si>
+    <t>Smartphone Xiaomi Poco F5 com processador Snapdragon 7+ Gen 2 Dual SIM 5G 8gb Ram 256gb Rom (Black)</t>
+  </si>
+  <si>
+    <t>R$ 149,99</t>
+  </si>
+  <si>
+    <t>Edifier W100T_GRBK Fone TWS - Fones sem fio, Bluetooth V5.1, Dark gray (cinza e preto)</t>
+  </si>
+  <si>
+    <t>R$ 1.869,90</t>
   </si>
 </sst>
 </file>
@@ -645,7 +930,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -758,7 +1043,7 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -766,10 +1051,10 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -934,7 +1219,7 @@
         <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -942,10 +1227,10 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
         <v>53</v>
-      </c>
-      <c r="C28" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -953,10 +1238,10 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" t="s">
         <v>55</v>
-      </c>
-      <c r="C29" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -964,10 +1249,10 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
         <v>57</v>
-      </c>
-      <c r="C30" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -975,10 +1260,10 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
         <v>59</v>
-      </c>
-      <c r="C31" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -986,10 +1271,10 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
         <v>61</v>
-      </c>
-      <c r="C32" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -997,10 +1282,10 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
         <v>63</v>
-      </c>
-      <c r="C33" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1008,10 +1293,10 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" t="s">
         <v>65</v>
-      </c>
-      <c r="C34" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1019,10 +1304,10 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
         <v>67</v>
-      </c>
-      <c r="C35" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1030,10 +1315,10 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
         <v>69</v>
-      </c>
-      <c r="C36" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1199,6 +1484,556 @@
       </c>
       <c r="C51" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" t="s">
+        <v>123</v>
+      </c>
+      <c r="C64" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" t="s">
+        <v>124</v>
+      </c>
+      <c r="C65" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" t="s">
+        <v>128</v>
+      </c>
+      <c r="C67" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" t="s">
+        <v>132</v>
+      </c>
+      <c r="C69" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" t="s">
+        <v>134</v>
+      </c>
+      <c r="C70" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>138</v>
+      </c>
+      <c r="C72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" t="s">
+        <v>140</v>
+      </c>
+      <c r="C73" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" t="s">
+        <v>142</v>
+      </c>
+      <c r="C74" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" t="s">
+        <v>144</v>
+      </c>
+      <c r="C75" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" t="s">
+        <v>145</v>
+      </c>
+      <c r="C76" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" t="s">
+        <v>147</v>
+      </c>
+      <c r="C77" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" t="s">
+        <v>149</v>
+      </c>
+      <c r="C78" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" t="s">
+        <v>151</v>
+      </c>
+      <c r="C79" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" t="s">
+        <v>153</v>
+      </c>
+      <c r="C80" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" t="s">
+        <v>155</v>
+      </c>
+      <c r="C81" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" t="s">
+        <v>159</v>
+      </c>
+      <c r="C83" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
+        <v>161</v>
+      </c>
+      <c r="C84" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
+        <v>163</v>
+      </c>
+      <c r="C85" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
+        <v>165</v>
+      </c>
+      <c r="C86" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" t="s">
+        <v>167</v>
+      </c>
+      <c r="C87" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" t="s">
+        <v>168</v>
+      </c>
+      <c r="C88" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" t="s">
+        <v>170</v>
+      </c>
+      <c r="C89" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" t="s">
+        <v>172</v>
+      </c>
+      <c r="C90" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" t="s">
+        <v>174</v>
+      </c>
+      <c r="C91" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92" t="s">
+        <v>176</v>
+      </c>
+      <c r="C92" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" t="s">
+        <v>178</v>
+      </c>
+      <c r="C93" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" t="s">
+        <v>180</v>
+      </c>
+      <c r="C94" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95" t="s">
+        <v>182</v>
+      </c>
+      <c r="C95" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" t="s">
+        <v>184</v>
+      </c>
+      <c r="C96" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97" t="s">
+        <v>186</v>
+      </c>
+      <c r="C97" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98" t="s">
+        <v>187</v>
+      </c>
+      <c r="C98" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99" t="s">
+        <v>189</v>
+      </c>
+      <c r="C99" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" t="s">
+        <v>191</v>
+      </c>
+      <c r="C100" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>3</v>
+      </c>
+      <c r="B101" t="s">
+        <v>193</v>
+      </c>
+      <c r="C101" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>